<commit_message>
Add worker schedule functionality and UI components
- Implemented worker schedule generation in main.py.
- Enhanced app.py to include a scrollable UI for worker schedules.
- Added HorarioTrabajadoresTreeview class for displaying weekly schedules.
- Updated imports to include new UI components.
</commit_message>
<xml_diff>
--- a/parametros_turnos_semana-new.xlsx
+++ b/parametros_turnos_semana-new.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000"/>
+    <workbookView windowWidth="20148" windowHeight="4356"/>
   </bookViews>
   <sheets>
     <sheet name="Parámetros" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
     <t>Turno (A o B)</t>
   </si>
   <si>
-    <t>A</t>
+    <t>B</t>
   </si>
   <si>
     <t/>
@@ -91,7 +91,7 @@
     <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,13 +103,6 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -709,152 +702,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -877,18 +870,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1243,7 +1224,7 @@
   <dimension ref="B2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -1265,7 +1246,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="4">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -1273,7 +1254,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:3">
@@ -1361,13 +1342,13 @@
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="3"/>
-      <c r="C12" s="12">
+      <c r="C12" s="9">
         <v>120</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="9">
         <v>220</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="10">
         <v>300</v>
       </c>
     </row>
@@ -1375,13 +1356,13 @@
       <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="11">
         <v>200</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="11">
         <v>280</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="5">
         <v>360</v>
       </c>
     </row>
@@ -1389,10 +1370,10 @@
       <c r="B14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="12">
         <v>220</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="12">
         <v>300</v>
       </c>
       <c r="E14" s="7">
@@ -1401,12 +1382,12 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="whole" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3 C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
+      <formula1>"A, B"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C4">
       <formula1>0</formula1>
       <formula2>999</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
-      <formula1>"A, B"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:E14">
       <formula1>0</formula1>

</xml_diff>

<commit_message>
Add shift scheduling functionality and update UI to display shift timings
</commit_message>
<xml_diff>
--- a/parametros_turnos_semana-new.xlsx
+++ b/parametros_turnos_semana-new.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20148" windowHeight="4356"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Parámetros" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Parámetro</t>
   </si>
@@ -44,7 +44,7 @@
     <t>Turno (A o B)</t>
   </si>
   <si>
-    <t>B</t>
+    <t>A</t>
   </si>
   <si>
     <t/>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Jueves</t>
+  </si>
+  <si>
+    <t>Viernes</t>
   </si>
   <si>
     <t>Sábado</t>
@@ -1224,7 +1227,7 @@
   <dimension ref="B2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -1246,7 +1249,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="4">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -1317,13 +1320,13 @@
         <v>13</v>
       </c>
       <c r="C10" s="9">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="D10" s="9">
         <v>160</v>
       </c>
       <c r="E10" s="10">
-        <v>200</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="2:5">
@@ -1331,53 +1334,55 @@
         <v>14</v>
       </c>
       <c r="C11" s="11">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D11" s="11">
-        <v>170</v>
+        <v>50</v>
       </c>
       <c r="E11" s="5">
         <v>220</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C12" s="9">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="D12" s="9">
-        <v>220</v>
+        <v>100</v>
       </c>
       <c r="E12" s="10">
-        <v>300</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" s="11">
+        <v>400</v>
+      </c>
+      <c r="D13" s="11">
         <v>200</v>
       </c>
-      <c r="D13" s="11">
-        <v>280</v>
-      </c>
       <c r="E13" s="5">
-        <v>360</v>
+        <v>500</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" s="12">
-        <v>220</v>
+        <v>400</v>
       </c>
       <c r="D14" s="12">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="E14" s="7">
-        <v>400</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>